<commit_message>
Initial commit of football analysis system
</commit_message>
<xml_diff>
--- a/game flow/Bundesliga_GameFlow.xlsx
+++ b/game flow/Bundesliga_GameFlow.xlsx
@@ -477,22 +477,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.657439446366782</v>
+        <v>5.686688311688312</v>
       </c>
       <c r="C2" t="n">
-        <v>8.809773123909249</v>
+        <v>8.697986577181208</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8115172554625281</v>
+        <v>0.8096501572327044</v>
       </c>
       <c r="E2" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2" t="n">
-        <v>0.04870084757537863</v>
+        <v>0.04943170354428677</v>
       </c>
       <c r="G2" t="n">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3">
@@ -527,97 +527,97 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4.598709677419355</v>
+        <v>4.584882280049566</v>
       </c>
       <c r="C4" t="n">
-        <v>8.123430962343097</v>
+        <v>8.150495049504951</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5668305057872205</v>
+        <v>0.5480639856480789</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
-        <v>0.08548387096774193</v>
+        <v>0.0842441740565065</v>
       </c>
       <c r="G4" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>VfB Stuttgart</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.919540229885057</v>
+        <v>5.792957746478873</v>
       </c>
       <c r="C5" t="n">
-        <v>8.072124756335283</v>
+        <v>7.952768729641694</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6507310870947235</v>
+        <v>0.5308977846871357</v>
       </c>
       <c r="E5" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F5" t="n">
-        <v>0.05825951967856817</v>
+        <v>0.07214939168159955</v>
       </c>
       <c r="G5" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bayer 04 Leverkusen</t>
+          <t>VfB Stuttgart</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5.888524590163934</v>
+        <v>4.919540229885057</v>
       </c>
       <c r="C6" t="n">
-        <v>10.74131274131274</v>
+        <v>8.072124756335283</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6220499372933531</v>
+        <v>0.6506866734486266</v>
       </c>
       <c r="E6" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
-        <v>0.05697272068882273</v>
+        <v>0.05817351598173516</v>
       </c>
       <c r="G6" t="n">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Bayer 04 Leverkusen</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5.943368107302534</v>
+        <v>5.888524590163934</v>
       </c>
       <c r="C7" t="n">
-        <v>7.996592844974447</v>
+        <v>10.74131274131274</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5294671689989235</v>
+        <v>0.6220499372933531</v>
       </c>
       <c r="E7" t="n">
         <v>18</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0716673220605584</v>
+        <v>0.05697272068882273</v>
       </c>
       <c r="G7" t="n">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
@@ -667,7 +667,7 @@
         <v>0.07637208401897203</v>
       </c>
       <c r="G9" t="n">
-        <v>-8</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="10">
@@ -692,7 +692,7 @@
         <v>0.134473606605721</v>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -702,22 +702,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6.505766062602965</v>
+        <v>6.455538221528861</v>
       </c>
       <c r="C11" t="n">
-        <v>9.192118226600986</v>
+        <v>8.92824074074074</v>
       </c>
       <c r="D11" t="n">
-        <v>0.452226481863757</v>
+        <v>0.4514075541094921</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
-        <v>0.07665630232001913</v>
+        <v>0.07709985062622084</v>
       </c>
       <c r="G11" t="n">
-        <v>-3</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="12">
@@ -767,7 +767,7 @@
         <v>0.07307482250136538</v>
       </c>
       <c r="G13" t="n">
-        <v>-8</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="14">
@@ -792,7 +792,7 @@
         <v>0.08279445727482679</v>
       </c>
       <c r="G14" t="n">
-        <v>-26</v>
+        <v>-27</v>
       </c>
     </row>
     <row r="15">
@@ -817,7 +817,7 @@
         <v>0.1088957055214724</v>
       </c>
       <c r="G15" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="16">
@@ -883,7 +883,7 @@
         <v>8.925000000000001</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4465770953294946</v>
+        <v>0.4466342462247249</v>
       </c>
       <c r="E18" t="n">
         <v>13</v>

</xml_diff>